<commit_message>
top 3 & rating
</commit_message>
<xml_diff>
--- a/public/services.xlsx
+++ b/public/services.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>artlib</t>
   </si>
@@ -39,6 +39,36 @@
   </si>
   <si>
     <t>La Dame à l’hermine est une peinture à l'huile sur panneau de bois de 54 × 39 cm réalisée par Léonard de Vinci à Milan, en 1488.</t>
+  </si>
+  <si>
+    <t>La Joconde</t>
+  </si>
+  <si>
+    <t>classique</t>
+  </si>
+  <si>
+    <t>Lisa, aussi connue sous le nom de Mona Lisa, Lisa di Antonio Maria Gherardini et de Lisa del Giocondo en italien, est un membre de la famille Gherardini de Florence</t>
+  </si>
+  <si>
+    <t>Gustav Klimt</t>
+  </si>
+  <si>
+    <t>Gustav Klimt, né le 14 juillet 1862 à Baumgarten en Autriche et mort le 6 février 1918 à Vienne.</t>
+  </si>
+  <si>
+    <t>La Nuit étoilée</t>
+  </si>
+  <si>
+    <t>paysages</t>
+  </si>
+  <si>
+    <t>La Nuit étoilée est une peinture de l'artiste peintre postimpressionniste néerlandais Vincent van Gogh.</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>regeprgoerrtre</t>
   </si>
 </sst>
 </file>
@@ -378,7 +408,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -418,6 +448,74 @@
       </c>
       <c r="E2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>410.0</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>466.0</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>200.0</v>
+      </c>
+      <c r="C5">
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>120.0</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>